<commit_message>
Variety Matters Redux 업데이트
#841
</commit_message>
<xml_diff>
--- a/Data/Variety Matters Redux - 3044059819/3044059819.xlsx
+++ b/Data/Variety Matters Redux - 3044059819/3044059819.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\Variety Matters Redux - 3044059819\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A025E5D3-1DE1-4468-BB59-D954A0869711}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E1365A-6656-45DD-89BA-F907EEDD3167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,18 +53,12 @@
     <t>Korean (한국어) [Translation]</t>
   </si>
   <si>
-    <t>VarietyMatters.FoodVariety_NeedDef+FoodVariety.label</t>
-  </si>
-  <si>
     <t>FoodVariety.label</t>
   </si>
   <si>
     <t>variety</t>
   </si>
   <si>
-    <t>VarietyMatters.FoodVariety_NeedDef+FoodVariety.description</t>
-  </si>
-  <si>
     <t>FoodVariety.description</t>
   </si>
   <si>
@@ -152,286 +146,305 @@
     <t>NeedFoodVariety.stages.3.label</t>
   </si>
   <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.3.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.3.description</t>
+  </si>
+  <si>
+    <t>The variety here is so scarce, it's hard to call it a meal.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.4.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.4.label</t>
+  </si>
+  <si>
+    <t>limited menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.4.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.4.description</t>
+  </si>
+  <si>
+    <t>Choices are limited. It's getting harder to enjoy meals.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.5.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.5.label</t>
+  </si>
+  <si>
+    <t>below average menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.5.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.5.description</t>
+  </si>
+  <si>
+    <t>The food is unremarkable, just enough to avoid monotony.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.6.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.6.label</t>
+  </si>
+  <si>
+    <t>average menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.6.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.6.description</t>
+  </si>
+  <si>
+    <t>It's an ordinary spread, nothing special, but not too bad either.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.7.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.7.label</t>
+  </si>
+  <si>
+    <t>above average menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.7.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.7.description</t>
+  </si>
+  <si>
+    <t>A decent variety that sometimes brings a pleasant surprise.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.8.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.8.label</t>
+  </si>
+  <si>
+    <t>good menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.8.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.8.description</t>
+  </si>
+  <si>
+    <t>The selection is quite satisfying, with a few favorites always around.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.9.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.9.label</t>
+  </si>
+  <si>
+    <t>great menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.9.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.9.description</t>
+  </si>
+  <si>
+    <t>There's always something interesting to try. Meals are delightful.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.10.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.10.label</t>
+  </si>
+  <si>
+    <t>excellent menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.10.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.10.description</t>
+  </si>
+  <si>
+    <t>A fantastic range of choices. Every meal is an adventure.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.11.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.11.label</t>
+  </si>
+  <si>
+    <t>exceptional menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.11.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.11.description</t>
+  </si>
+  <si>
+    <t>It's like dining at a top-notch restaurant every day. Absolutely superb.</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.12.label</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.12.label</t>
+  </si>
+  <si>
+    <t>overwhelming menu</t>
+  </si>
+  <si>
+    <t>ThoughtDef+NeedFoodVariety.stages.12.description</t>
+  </si>
+  <si>
+    <t>NeedFoodVariety.stages.12.description</t>
+  </si>
+  <si>
+    <t>The variety is staggering, almost too much to take in!</t>
+  </si>
+  <si>
+    <t>식사 다양성</t>
+  </si>
+  <si>
+    <t>오랜만에 먹어봤어.</t>
+  </si>
+  <si>
+    <t>새로운 맛 경험</t>
+  </si>
+  <si>
+    <t>식사하기가 힘들어.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>단조로운 식단이야.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>평범한 식단이야.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>꽤 다양한 선택지가 있어.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>만족스러운 선택지야.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>식사시간이 너무 즐거워.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다양한 선택지가 있어. 매 식사가 모험이야.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>매일 레스토랑에서 식사하는 것 같아.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedDef</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>다양한 식단은 건강하고 행복한 삶을 만듭니다. 기대 이상의 다양성을 제공하면 긍정적인 생각을 유발하며, 충분한 다양성을 제공하지 않으면 부정적인 생각을 유발할 수 있습니다.</t>
+  </si>
+  <si>
+    <t>특별하지 않지만 그렇다고 나쁘진 않아.</t>
+  </si>
+  <si>
+    <t>NeedDef+FoodVariety.label</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedDef+FoodVariety.description</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>먹을 게 없어. 살려줘.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>또 그걸 먹을 수 없어.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>여긴 선택지가 너무 제한적이야. 이걸 밥이라고 부를 수도 없겠어.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리 정착지는 정말 최고야.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>한정된 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균 이하 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>보통 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>평균 이상 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>좋은 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>훌륭한 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>뛰어난 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>우수한 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>찬란한 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>황폐한 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>궁핍한 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>빈곤한 식단</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>scarce menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.3.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.3.description</t>
-  </si>
-  <si>
-    <t>The variety here is so scarce, it's hard to call it a meal.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.4.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.4.label</t>
-  </si>
-  <si>
-    <t>limited menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.4.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.4.description</t>
-  </si>
-  <si>
-    <t>Choices are limited. It's getting harder to enjoy meals.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.5.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.5.label</t>
-  </si>
-  <si>
-    <t>below average menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.5.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.5.description</t>
-  </si>
-  <si>
-    <t>The food is unremarkable, just enough to avoid monotony.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.6.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.6.label</t>
-  </si>
-  <si>
-    <t>average menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.6.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.6.description</t>
-  </si>
-  <si>
-    <t>It's an ordinary spread, nothing special, but not too bad either.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.7.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.7.label</t>
-  </si>
-  <si>
-    <t>above average menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.7.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.7.description</t>
-  </si>
-  <si>
-    <t>A decent variety that sometimes brings a pleasant surprise.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.8.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.8.label</t>
-  </si>
-  <si>
-    <t>good menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.8.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.8.description</t>
-  </si>
-  <si>
-    <t>The selection is quite satisfying, with a few favorites always around.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.9.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.9.label</t>
-  </si>
-  <si>
-    <t>great menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.9.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.9.description</t>
-  </si>
-  <si>
-    <t>There's always something interesting to try. Meals are delightful.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.10.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.10.label</t>
-  </si>
-  <si>
-    <t>excellent menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.10.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.10.description</t>
-  </si>
-  <si>
-    <t>A fantastic range of choices. Every meal is an adventure.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.11.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.11.label</t>
-  </si>
-  <si>
-    <t>exceptional menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.11.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.11.description</t>
-  </si>
-  <si>
-    <t>It's like dining at a top-notch restaurant every day. Absolutely superb.</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.12.label</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.12.label</t>
-  </si>
-  <si>
-    <t>overwhelming menu</t>
-  </si>
-  <si>
-    <t>ThoughtDef+NeedFoodVariety.stages.12.description</t>
-  </si>
-  <si>
-    <t>NeedFoodVariety.stages.12.description</t>
-  </si>
-  <si>
-    <t>The variety is staggering, almost too much to take in!</t>
-  </si>
-  <si>
-    <t>식사 다양성</t>
-  </si>
-  <si>
-    <t>찬란한 메뉴</t>
-  </si>
-  <si>
-    <t>우수한 메뉴</t>
-  </si>
-  <si>
-    <t>뛰어난 메뉴</t>
-  </si>
-  <si>
-    <t>훌륭한 메뉴</t>
-  </si>
-  <si>
-    <t>좋은 메뉴</t>
-  </si>
-  <si>
-    <t>평균 이상 메뉴</t>
-  </si>
-  <si>
-    <t>보통 메뉴</t>
-  </si>
-  <si>
-    <t>평균 이하 메뉴</t>
-  </si>
-  <si>
-    <t>한정된 메뉴</t>
-  </si>
-  <si>
-    <t>다채로운 메뉴 부재</t>
-  </si>
-  <si>
-    <t>한가지 메뉴</t>
-  </si>
-  <si>
-    <t>식단 고갈</t>
-  </si>
-  <si>
-    <t>오랜만에 먹어봤어.</t>
-  </si>
-  <si>
-    <t>새로운 맛 경험</t>
-  </si>
-  <si>
-    <t>먹고 싶지 않은 메뉴</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>선택지가 없어.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>식사가 고통스러워.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>또 그걸 먹을 순 없어.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>식사하기가 힘들어.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>단조로운 식단이야.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>평범한 식단이야.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>특별하진 않아도 나쁘진 않아.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>꽤 다양한 선택지가 있어.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>만족스러운 선택지야.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>식사시간이 너무 즐거워.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다양한 선택지가 있어. 매 식사가 모험이야.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>매일 레스토랑에서 식사하는 것 같아.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>우리 정착지는 천국이야.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedDef</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>다양한 식단은 건강하고 행복한 삶을 만듭니다. 기대 이상의 다양성을 제공하면 긍정적인 생각을 유발하며, 충분한 다양성을 제공하지 않으면 부정적인 생각을 유발할 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모자란 식단</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -792,12 +805,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="61.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="87.26953125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="59.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="61.54296875" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
@@ -823,512 +836,512 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>116</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>117</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>118</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>